<commit_message>
Most of the report done
Needs summary, answering a couple of questions, proofreading
</commit_message>
<xml_diff>
--- a/src/unitTests/project3analysis.xlsx
+++ b/src/unitTests/project3analysis.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9700" windowHeight="560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9700" windowHeight="560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table Size 97" sheetId="1" r:id="rId1"/>
     <sheet name="Table Size 7919" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="correlator errorSums" sheetId="3" r:id="rId3"/>
+    <sheet name="correlator adt times" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -365,12 +367,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -385,9 +399,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,6 +491,49 @@
         <a:xfrm>
           <a:off x="7924800" y="552450"/>
           <a:ext cx="8495238" cy="6285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>149312</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>188723</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6854912" y="0"/>
+          <a:ext cx="7354611" cy="5111750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -751,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -979,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B45"/>
+  <dimension ref="B2:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B45"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1057,132 +1116,155 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B35" t="s">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B35" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B44" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>79</v>
       </c>
@@ -1196,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B25:N49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1319,4 +1401,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>